<commit_message>
work on asset sheet in progress
</commit_message>
<xml_diff>
--- a/Chapter 11/Audio Asset Tracking Sheet EXAMPLE.xlsx
+++ b/Chapter 11/Audio Asset Tracking Sheet EXAMPLE.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbolt\Desktop\Reaper\Elevate-your-audio-production-with-Reaper\Chapter 11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbolt\Documents\GitHub\Elevate-your-audio-production-with-Reaper\Chapter 11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D483CD6E-386A-45C6-B30E-9F114AD8BA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50D8BDF-5B37-402A-8207-506493BD05F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15370" xr2:uid="{D58FA421-E253-4084-844C-17AE215338B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D58FA421-E253-4084-844C-17AE215338B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ASSET LIST" sheetId="1" r:id="rId1"/>
+    <sheet name="Dropdown Sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,9 +36,116 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t>&lt;Project Title&gt;</t>
+  </si>
+  <si>
+    <t>Audio Asset Tracking</t>
+  </si>
+  <si>
+    <t>CONFIDENTIAL! DO NOT SHARE!</t>
+  </si>
+  <si>
+    <t>&lt;Your Name&gt;</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Asset Name</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>References / Inspo</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Recording</t>
+  </si>
+  <si>
+    <t>Drafting</t>
+  </si>
+  <si>
+    <t>Ready for Review</t>
+  </si>
+  <si>
+    <t>Iterating</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Waiting for Approal</t>
+  </si>
+  <si>
+    <t>Designing</t>
+  </si>
+  <si>
+    <t>&lt; Status Dropdown</t>
+  </si>
+  <si>
+    <t>(add or remove options from column).</t>
+  </si>
+  <si>
+    <t>Cinematics</t>
+  </si>
+  <si>
+    <t>&lt; Category Dropdown</t>
+  </si>
+  <si>
+    <t>(add or remove options from column)</t>
+  </si>
+  <si>
+    <t>Ambience-AMB</t>
+  </si>
+  <si>
+    <t>Foley-FOLY</t>
+  </si>
+  <si>
+    <t>Vehicles-VEH</t>
+  </si>
+  <si>
+    <t>Weapons-WEAP</t>
+  </si>
+  <si>
+    <t>Abilities_ABL</t>
+  </si>
+  <si>
+    <t>Voice-VOX</t>
+  </si>
+  <si>
+    <t>Rev 1</t>
+  </si>
+  <si>
+    <t>Rev 2</t>
+  </si>
+  <si>
+    <t>Rev 3</t>
+  </si>
+  <si>
+    <t>Rev 4</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,19 +153,130 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -66,13 +285,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -402,14 +668,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE8F6CCF-36E8-4105-976F-5E70D42EF823}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="70.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="10" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="11" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="D3" s="14"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Approval">
+      <formula>NOT(ISERROR(SEARCH("Approval",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Approval+'ASSET LIST'!$A$7">
+      <formula>NOT(ISERROR(SEARCH("Approval+'ASSET LIST'!$A$7",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Asset Status" prompt="Select Asset Status / Staging" xr:uid="{7EC83479-8D6E-43AB-B44C-656D84995F2C}">
+          <x14:formula1>
+            <xm:f>'Dropdown Sources'!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Audio Asset Category" prompt="Select Category" xr:uid="{BE5F6B74-78B4-41D1-B76C-C800523739D6}">
+          <x14:formula1>
+            <xm:f>'Dropdown Sources'!$C:$C</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA3D107-9E79-4124-94BE-C596802C55ED}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Audio Asset Tracking Sheet EXAMPLE.xlsx
</commit_message>
<xml_diff>
--- a/Chapter 11/Audio Asset Tracking Sheet EXAMPLE.xlsx
+++ b/Chapter 11/Audio Asset Tracking Sheet EXAMPLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbolt\Documents\GitHub\Elevate-your-audio-production-with-Reaper\Chapter 11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50D8BDF-5B37-402A-8207-506493BD05F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0576751E-83A3-4869-9EC2-4D12F52EC619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D58FA421-E253-4084-844C-17AE215338B6}"/>
   </bookViews>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>&lt;Project Title&gt;</t>
   </si>
@@ -139,13 +137,16 @@
   </si>
   <si>
     <t>Rev 4</t>
+  </si>
+  <si>
+    <t>Variations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +199,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -285,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -295,22 +303,25 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,41 +679,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE8F6CCF-36E8-4105-976F-5E70D42EF823}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D5" sqref="D5"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="70.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.77734375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="3" width="20.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="70.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="11" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="11" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -712,32 +723,35 @@
       <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Approval">
-      <formula>NOT(ISERROR(SEARCH("Approval",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Approval",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
+  <conditionalFormatting sqref="E3">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Approval+'ASSET LIST'!$A$7">
-      <formula>NOT(ISERROR(SEARCH("Approval+'ASSET LIST'!$A$7",D3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Approval+'ASSET LIST'!$A$7",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -749,7 +763,7 @@
           <x14:formula1>
             <xm:f>'Dropdown Sources'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>D3</xm:sqref>
+          <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Audio Asset Category" prompt="Select Category" xr:uid="{BE5F6B74-78B4-41D1-B76C-C800523739D6}">
           <x14:formula1>

</xml_diff>